<commit_message>
added name description as a function input for plot_nodal_accelerations and write_nodal_accelerations_to_excel
</commit_message>
<xml_diff>
--- a/nodal_accels.xlsx
+++ b/nodal_accels.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>181</t>
+    <t>181 - Node 1</t>
   </si>
   <si>
     <t>Frequency (Hz)</t>
@@ -423,13 +423,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>0.7845547795295715</v>
+        <v>0.785</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>5.070035934448242</v>
+        <v>5.070000171661377</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -446,13 +446,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4">
-        <v>0.8281410932540894</v>
+        <v>0.828</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>8.868691444396973</v>
+        <v>8.869999885559082</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -469,13 +469,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5">
-        <v>0.8717275261878967</v>
+        <v>0.872</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>16.69664001464844</v>
+        <v>16.70000076293945</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -492,13 +492,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6">
-        <v>0.9153138995170593</v>
+        <v>0.915</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>8.328123092651367</v>
+        <v>8.329999923706055</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -515,13 +515,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7">
-        <v>0.9589002728462219</v>
+        <v>0.959</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7">
-        <v>4.552709579467773</v>
+        <v>4.550000190734863</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -544,7 +544,7 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.03315182402729988</v>
+        <v>0.02999999932944775</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -567,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <v>0.02332929708063602</v>
+        <v>0.01999999955296516</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -590,7 +590,7 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0.01748516410589218</v>
+        <v>0.01999999955296516</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.0137171559035778</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -636,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.01114008110016584</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -659,7 +659,7 @@
         <v>0</v>
       </c>
       <c r="C13">
-        <v>0.009295632131397724</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -682,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0.007926891557872295</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.006880656350404024</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -728,7 +728,7 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0.006060936953872442</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0.005405089817941189</v>
+        <v>0.009999999776482582</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -774,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="C18">
-        <v>0.004870819859206676</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>0</v>
       </c>
       <c r="C19">
-        <v>0.004428728949278593</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -820,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="C20">
-        <v>0.004057866986840963</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -843,7 +843,7 @@
         <v>0</v>
       </c>
       <c r="C21">
-        <v>0.003742972621694207</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -866,7 +866,7 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0.003472713055089116</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -889,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="C23">
-        <v>0.00323852663859725</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="C24">
-        <v>0.003033845452591777</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -935,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="C25">
-        <v>0.002853560028597713</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0.002693646354600787</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -981,7 +981,7 @@
         <v>0</v>
       </c>
       <c r="C27">
-        <v>0.002550896955654025</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="C28">
-        <v>0.00242272880859673</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -1027,7 +1027,7 @@
         <v>0</v>
       </c>
       <c r="C29">
-        <v>0.002307043178007007</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -1050,7 +1050,7 @@
         <v>0</v>
       </c>
       <c r="C30">
-        <v>0.002202116884291172</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="C31">
-        <v>0.002106525003910065</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1096,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="C32">
-        <v>0.002019079867750406</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         <v>0</v>
       </c>
       <c r="C33">
-        <v>0.001938784262165427</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
       <c r="C34">
-        <v>0.001864795689471066</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -1165,7 +1165,7 @@
         <v>0</v>
       </c>
       <c r="C35">
-        <v>0.001796397496946156</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -1188,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="C36">
-        <v>0.001732976757921278</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="C37">
-        <v>0.001674006343819201</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1234,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="C38">
-        <v>0.001619030837900937</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="C39">
-        <v>0.00156765419524163</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1280,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="C40">
-        <v>0.001519531127996743</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="C41">
-        <v>0.001474358956329525</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -1326,7 +1326,7 @@
         <v>0</v>
       </c>
       <c r="C42">
-        <v>0.001431871671229601</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1349,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="C43">
-        <v>0.001391834113746881</v>
+        <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1372,7 +1372,7 @@
         <v>0</v>
       </c>
       <c r="C44">
-        <v>0.001354037551209331</v>
+        <v>0</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45">
-        <v>41.20682907104492</v>
+        <v>41.207</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
       <c r="C45">
-        <v>0.001346482429653406</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1418,7 +1418,7 @@
         <v>0</v>
       </c>
       <c r="C46">
-        <v>0.001318296766839921</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1441,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="C47">
-        <v>0.001284446334466338</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1458,13 +1458,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48">
-        <v>43.49610137939453</v>
+        <v>43.496</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>0.001268308260478079</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -1487,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="C49">
-        <v>0.001252337940968573</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -1510,7 +1510,7 @@
         <v>0</v>
       </c>
       <c r="C50">
-        <v>0.001221838872879744</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1527,13 +1527,13 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51">
-        <v>45.78536987304688</v>
+        <v>45.785</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
       <c r="C51">
-        <v>0.001198935671709478</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="C52">
-        <v>0.00119282933883369</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1579,7 +1579,7 @@
         <v>0</v>
       </c>
       <c r="C53">
-        <v>0.001165200956165791</v>
+        <v>0</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1602,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="C54">
-        <v>0.001138856168836355</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -1619,13 +1619,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55">
-        <v>48.07463836669922</v>
+        <v>48.075</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
       <c r="C55">
-        <v>0.001136938924901187</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -1648,7 +1648,7 @@
         <v>0</v>
       </c>
       <c r="C56">
-        <v>0.001113706617616117</v>
+        <v>0</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -1671,7 +1671,7 @@
         <v>0</v>
       </c>
       <c r="C57">
-        <v>0.001089671044610441</v>
+        <v>0</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -1688,13 +1688,13 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>50.36391067504883</v>
+        <v>50.364</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
       <c r="C58">
-        <v>0.001081186230294406</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -1717,7 +1717,7 @@
         <v>0</v>
       </c>
       <c r="C59">
-        <v>0.001066676224581897</v>
+        <v>0</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -1740,7 +1740,7 @@
         <v>0</v>
       </c>
       <c r="C60">
-        <v>0.001044654869474471</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="C61">
-        <v>0.001023545628413558</v>
+        <v>0</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -1786,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="C62">
-        <v>0.001003292039968073</v>
+        <v>0</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1809,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="C63">
-        <v>0.0009838424157351255</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -1832,7 +1832,7 @@
         <v>0</v>
       </c>
       <c r="C64">
-        <v>0.0009651491418480873</v>
+        <v>0</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -1855,7 +1855,7 @@
         <v>0</v>
       </c>
       <c r="C65">
-        <v>0.000947168271522969</v>
+        <v>0</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="C66">
-        <v>0.0009298592340201139</v>
+        <v>0</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -1901,7 +1901,7 @@
         <v>0</v>
       </c>
       <c r="C67">
-        <v>0.0009131844853982329</v>
+        <v>0</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
       <c r="C68">
-        <v>0.0008971093920990825</v>
+        <v>0</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -1947,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="C69">
-        <v>0.0008816015906631947</v>
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1970,7 +1970,7 @@
         <v>0</v>
       </c>
       <c r="C70">
-        <v>0.0008666312787681818</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -1993,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="C71">
-        <v>0.0008521705167368054</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -2016,7 +2016,7 @@
         <v>0</v>
       </c>
       <c r="C72">
-        <v>0.0008381934021599591</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>0</v>
       </c>
       <c r="C73">
-        <v>0.0008246757788583636</v>
+        <v>0</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -2062,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="C74">
-        <v>0.0008115950040519238</v>
+        <v>0</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="C75">
-        <v>0.0007989299483597279</v>
+        <v>0</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -2108,7 +2108,7 @@
         <v>0</v>
       </c>
       <c r="C76">
-        <v>0.0007866608211770654</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -2131,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="C77">
-        <v>0.0007747691124677658</v>
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2154,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="C78">
-        <v>0.0007632375927641988</v>
+        <v>0</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -2177,7 +2177,7 @@
         <v>0</v>
       </c>
       <c r="C79">
-        <v>0.0007520497310906649</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -2200,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="C80">
-        <v>0.0007411903352476656</v>
+        <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2223,7 +2223,7 @@
         <v>0</v>
       </c>
       <c r="C81">
-        <v>0.0007306449115276337</v>
+        <v>0</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -2246,7 +2246,7 @@
         <v>0</v>
       </c>
       <c r="C82">
-        <v>0.0007203998393379152</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -2269,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>0.0007104424294084311</v>
+        <v>0</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -2292,7 +2292,7 @@
         <v>0</v>
       </c>
       <c r="C84">
-        <v>0.0007007604581303895</v>
+        <v>0</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -2315,7 +2315,7 @@
         <v>0</v>
       </c>
       <c r="C85">
-        <v>0.0006913426332175732</v>
+        <v>0</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -2338,7 +2338,7 @@
         <v>0</v>
       </c>
       <c r="C86">
-        <v>0.0006821781280450523</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -2361,7 +2361,7 @@
         <v>0</v>
       </c>
       <c r="C87">
-        <v>0.0006732566980645061</v>
+        <v>0</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="C88">
-        <v>0.0006645687390118837</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -2407,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="C89">
-        <v>0.0006561051122844219</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -2430,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="C90">
-        <v>0.0006478570867329836</v>
+        <v>0</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -2453,7 +2453,7 @@
         <v>0</v>
       </c>
       <c r="C91">
-        <v>0.0006398164550773799</v>
+        <v>0</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -2476,7 +2476,7 @@
         <v>0</v>
       </c>
       <c r="C92">
-        <v>0.0006319755339063704</v>
+        <v>0</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -2499,7 +2499,7 @@
         <v>0</v>
       </c>
       <c r="C93">
-        <v>0.0006243267562240362</v>
+        <v>0</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -2522,7 +2522,7 @@
         <v>0</v>
       </c>
       <c r="C94">
-        <v>0.0006168631371110678</v>
+        <v>0</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -2545,7 +2545,7 @@
         <v>0</v>
       </c>
       <c r="C95">
-        <v>0.0006095779244787991</v>
+        <v>0</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -2568,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="C96">
-        <v>0.0006024647736921906</v>
+        <v>0</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -2591,7 +2591,7 @@
         <v>0</v>
       </c>
       <c r="C97">
-        <v>0.0005955175729468465</v>
+        <v>0</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -2614,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="C98">
-        <v>0.0005887305014766753</v>
+        <v>0</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -2637,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="C99">
-        <v>0.000582098204176873</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -2660,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="C100">
-        <v>0.0005756150931119919</v>
+        <v>0</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -2683,7 +2683,7 @@
         <v>0</v>
       </c>
       <c r="C101">
-        <v>0.0005692763952538371</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -2706,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="C102">
-        <v>0.000563077162951231</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -2729,7 +2729,7 @@
         <v>0</v>
       </c>
       <c r="C103">
-        <v>0.0005570129142142832</v>
+        <v>0</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -2752,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="C104">
-        <v>0.0005510792252607644</v>
+        <v>0</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -2775,7 +2775,7 @@
         <v>0</v>
       </c>
       <c r="C105">
-        <v>0.0005452717887237668</v>
+        <v>0</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -2798,7 +2798,7 @@
         <v>0</v>
       </c>
       <c r="C106">
-        <v>0.0005395866464823484</v>
+        <v>0</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -2821,7 +2821,7 @@
         <v>0</v>
       </c>
       <c r="C107">
-        <v>0.0005340200150385499</v>
+        <v>0</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -2844,7 +2844,7 @@
         <v>0</v>
       </c>
       <c r="C108">
-        <v>0.0005285680526867509</v>
+        <v>0</v>
       </c>
       <c r="D108">
         <v>0</v>

</xml_diff>